<commit_message>
Added more tables to the data dictionary
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haysa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{458C553F-CB08-40B7-91B4-3FDA43F54F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E528383-8A4B-4FDD-85F8-D8A980CC76C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
   </bookViews>
   <sheets>
     <sheet name="Role" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Team Admin" sheetId="8" r:id="rId5"/>
     <sheet name="Comp admin" sheetId="9" r:id="rId6"/>
     <sheet name="Match Official" sheetId="10" r:id="rId7"/>
+    <sheet name="Event booking" sheetId="11" r:id="rId8"/>
+    <sheet name="matchOfficialSelection" sheetId="12" r:id="rId9"/>
+    <sheet name="Match" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
   <si>
     <t>Key</t>
   </si>
@@ -163,6 +166,60 @@
   </si>
   <si>
     <t>An ID unique to each team admin</t>
+  </si>
+  <si>
+    <t>An ID unique to each booking</t>
+  </si>
+  <si>
+    <t>PK, FK</t>
+  </si>
+  <si>
+    <t>References the role ID</t>
+  </si>
+  <si>
+    <t>CompAdmin_ID</t>
+  </si>
+  <si>
+    <t>References the comp_admin ID</t>
+  </si>
+  <si>
+    <t>Team ID</t>
+  </si>
+  <si>
+    <t>References team ID</t>
+  </si>
+  <si>
+    <t>References the official selection table</t>
+  </si>
+  <si>
+    <t>Match Official ID</t>
+  </si>
+  <si>
+    <t>Match ID</t>
+  </si>
+  <si>
+    <t>References the match official selected</t>
+  </si>
+  <si>
+    <t>References the match ID</t>
+  </si>
+  <si>
+    <t>An ID unique to each match</t>
+  </si>
+  <si>
+    <t>selectionID</t>
+  </si>
+  <si>
+    <t>Selection ID</t>
+  </si>
+  <si>
+    <t>resultID</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>Referenced in role_id table</t>
   </si>
 </sst>
 </file>
@@ -522,10 +579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430BA5C4-9375-452D-AC95-638ADFDC1637}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +630,94 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21F66D-F8C0-434D-8A17-9B05CAE03D77}">
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="43.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -581,10 +726,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89383853-FD85-49A5-8CA3-D73C5E0405E4}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,6 +817,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3134A29A-D97E-4DC9-B445-824F51CC3799}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -815,6 +962,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D502AB1-48A8-44FF-AF00-D68D50C38B7E}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -880,10 +1028,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8559D0D4-9307-4B03-AE70-D0E674879CE4}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,7 +1079,15 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,10 +1096,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA88D118-22B4-4B9F-B65A-29B555017388}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,7 +1147,15 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -998,16 +1164,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119B9A4A-D93E-4E1C-BFB0-DE14987F36C9}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -1048,7 +1215,162 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D373D72A-ADE9-4F1E-BE71-D18BF2E63DA0}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932EF1F6-77F7-4C2A-9AB9-F143830512D7}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data dictionary is almost finished, Acc table still needs done
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haysa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C995BE-5C54-4824-9E50-C22F40BC0234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CDF6AC-8727-4808-B867-27A671DBFF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="15" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="20" activeTab="27" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
   </bookViews>
   <sheets>
     <sheet name="Role" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,18 @@
     <sheet name="Point" sheetId="18" r:id="rId14"/>
     <sheet name="Result" sheetId="19" r:id="rId15"/>
     <sheet name="Squad" sheetId="21" r:id="rId16"/>
+    <sheet name="Season" sheetId="22" r:id="rId17"/>
+    <sheet name="Competition" sheetId="24" r:id="rId18"/>
+    <sheet name="Team Entry" sheetId="25" r:id="rId19"/>
+    <sheet name="Grade" sheetId="26" r:id="rId20"/>
+    <sheet name="Team" sheetId="27" r:id="rId21"/>
+    <sheet name="Player_Team" sheetId="28" r:id="rId22"/>
+    <sheet name="Position" sheetId="29" r:id="rId23"/>
+    <sheet name="Accident Register" sheetId="30" r:id="rId24"/>
+    <sheet name="Injury Report" sheetId="31" r:id="rId25"/>
+    <sheet name="Injury Code" sheetId="32" r:id="rId26"/>
+    <sheet name="Acc Codes" sheetId="33" r:id="rId27"/>
+    <sheet name="ACC" sheetId="34" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="186">
   <si>
     <t>Key</t>
   </si>
@@ -87,12 +99,6 @@
     <t>PK, FK2</t>
   </si>
   <si>
-    <t>role_id</t>
-  </si>
-  <si>
-    <t>person_id</t>
-  </si>
-  <si>
     <t>The role ID referencing the role table</t>
   </si>
   <si>
@@ -183,9 +189,6 @@
     <t>References the role ID</t>
   </si>
   <si>
-    <t>CompAdmin_ID</t>
-  </si>
-  <si>
     <t>References the comp_admin ID</t>
   </si>
   <si>
@@ -210,9 +213,6 @@
     <t>An ID unique to each match</t>
   </si>
   <si>
-    <t>selectionID</t>
-  </si>
-  <si>
     <t>Selection ID</t>
   </si>
   <si>
@@ -222,24 +222,6 @@
     <t>Referenced in role_id table</t>
   </si>
   <si>
-    <t>FieldID</t>
-  </si>
-  <si>
-    <t>FacilityID</t>
-  </si>
-  <si>
-    <t>CompetitionID</t>
-  </si>
-  <si>
-    <t>PointID</t>
-  </si>
-  <si>
-    <t>SquadID</t>
-  </si>
-  <si>
-    <t>BookingID</t>
-  </si>
-  <si>
     <t>Refers to the match officials selected</t>
   </si>
   <si>
@@ -285,42 +267,24 @@
     <t>Address of the facility</t>
   </si>
   <si>
-    <t>FacilityAdminID</t>
-  </si>
-  <si>
     <t>Refers to the admin of the facility</t>
   </si>
   <si>
     <t>The contact number for the facility</t>
   </si>
   <si>
-    <t>RoleID</t>
-  </si>
-  <si>
     <t>Refers to the persons role</t>
   </si>
   <si>
     <t>refers to the facility worked at</t>
   </si>
   <si>
-    <t>matchID</t>
-  </si>
-  <si>
     <t>Refers the match</t>
   </si>
   <si>
-    <t>PlayerID</t>
-  </si>
-  <si>
-    <t>ResultID</t>
-  </si>
-  <si>
     <t>Refers to the player who scored the point</t>
   </si>
   <si>
-    <t>MatchID</t>
-  </si>
-  <si>
     <t>References the Field the game will be taking place on</t>
   </si>
   <si>
@@ -369,22 +333,292 @@
     <t>Is the player available to play</t>
   </si>
   <si>
-    <t>SeasonID</t>
-  </si>
-  <si>
     <t>Winner</t>
   </si>
   <si>
     <t>Team id of winner</t>
   </si>
   <si>
-    <t>entryID</t>
-  </si>
-  <si>
-    <t>playing</t>
-  </si>
-  <si>
     <t>array of player's ID's</t>
+  </si>
+  <si>
+    <t>players</t>
+  </si>
+  <si>
+    <t>entry ID</t>
+  </si>
+  <si>
+    <t>match ID</t>
+  </si>
+  <si>
+    <t>Season ID</t>
+  </si>
+  <si>
+    <t>Result ID</t>
+  </si>
+  <si>
+    <t>Player ID</t>
+  </si>
+  <si>
+    <t>FacilityAdmin ID</t>
+  </si>
+  <si>
+    <t>Facility ID</t>
+  </si>
+  <si>
+    <t>Squad ID</t>
+  </si>
+  <si>
+    <t>Competition ID</t>
+  </si>
+  <si>
+    <t>selection ID</t>
+  </si>
+  <si>
+    <t>Field ID</t>
+  </si>
+  <si>
+    <t>CompAdmin ID</t>
+  </si>
+  <si>
+    <t>Date of booking</t>
+  </si>
+  <si>
+    <t>Date of game</t>
+  </si>
+  <si>
+    <t>The date the booking was made</t>
+  </si>
+  <si>
+    <t>The date the booking was made for</t>
+  </si>
+  <si>
+    <t>date/time</t>
+  </si>
+  <si>
+    <t>role ID</t>
+  </si>
+  <si>
+    <t>person ID</t>
+  </si>
+  <si>
+    <t>A list of the players playing in the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Grade ID ???</t>
+  </si>
+  <si>
+    <t>TeamEntry ID</t>
+  </si>
+  <si>
+    <t>Grade ID</t>
+  </si>
+  <si>
+    <t>Refers to the team playing</t>
+  </si>
+  <si>
+    <t>Refers to the competition the team are playing in</t>
+  </si>
+  <si>
+    <t>Refers to the teams grade</t>
+  </si>
+  <si>
+    <t>Refers to the match being played</t>
+  </si>
+  <si>
+    <t>Refers to the teams entry to the match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refers to the results </t>
+  </si>
+  <si>
+    <t>Refers to the competition the season is part of</t>
+  </si>
+  <si>
+    <t>Refers to the match the suqad is playing in</t>
+  </si>
+  <si>
+    <t>Refers to the squads entry</t>
+  </si>
+  <si>
+    <t>Refers to the points scored in the game</t>
+  </si>
+  <si>
+    <t>Refers to the season the results are for</t>
+  </si>
+  <si>
+    <t>The winner of the game</t>
+  </si>
+  <si>
+    <t>TeamEntery ID</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>The grade of the team</t>
+  </si>
+  <si>
+    <t>Refers to the team at the time of entry</t>
+  </si>
+  <si>
+    <t>TeamAdmin ID</t>
+  </si>
+  <si>
+    <t>Refers to the admin of the team</t>
+  </si>
+  <si>
+    <t>PlayerTeam ID</t>
+  </si>
+  <si>
+    <t>Refers to a player</t>
+  </si>
+  <si>
+    <t>The name of the team</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>The home grounds of the team</t>
+  </si>
+  <si>
+    <t>Team  ID</t>
+  </si>
+  <si>
+    <t>Position ID</t>
+  </si>
+  <si>
+    <t>Refers to the players position</t>
+  </si>
+  <si>
+    <t>Refers to the player</t>
+  </si>
+  <si>
+    <t>Refers to the team the player plays for</t>
+  </si>
+  <si>
+    <t>Player Team ID</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>A position in a team</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to </t>
+  </si>
+  <si>
+    <t>Injury Report ID</t>
+  </si>
+  <si>
+    <t>An ID unique to the register</t>
+  </si>
+  <si>
+    <t>An ID unique to each position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An ID unique to each </t>
+  </si>
+  <si>
+    <t>An ID unique to each team</t>
+  </si>
+  <si>
+    <t>An ID unique to each grade</t>
+  </si>
+  <si>
+    <t>An ID unique to each team entry</t>
+  </si>
+  <si>
+    <t>An ID unique to each competiton</t>
+  </si>
+  <si>
+    <t>An ID unique to each season</t>
+  </si>
+  <si>
+    <t>An ID unique to each squad</t>
+  </si>
+  <si>
+    <t>An ID unique to the results</t>
+  </si>
+  <si>
+    <t>An ID unique to the points scored</t>
+  </si>
+  <si>
+    <t>An ID unique to each sports facility</t>
+  </si>
+  <si>
+    <t>An ID unique to each field</t>
+  </si>
+  <si>
+    <t>An ID unique to each selection</t>
+  </si>
+  <si>
+    <t>An ID unique to each facility admin</t>
+  </si>
+  <si>
+    <t>An ID unique to each role</t>
+  </si>
+  <si>
+    <t>Refers to the Injury report who can access the register</t>
+  </si>
+  <si>
+    <t>An ID unique to the report</t>
+  </si>
+  <si>
+    <t>Injury Code ID</t>
+  </si>
+  <si>
+    <t>register ID</t>
+  </si>
+  <si>
+    <t>Refers to the registery the report is being made on</t>
+  </si>
+  <si>
+    <t>Reporter</t>
+  </si>
+  <si>
+    <t>Injured</t>
+  </si>
+  <si>
+    <t>Who is filling out the report</t>
+  </si>
+  <si>
+    <t>Who was injured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes </t>
+  </si>
+  <si>
+    <t>Notes about the injury. How it happened etc</t>
+  </si>
+  <si>
+    <t>Acc Code ID</t>
+  </si>
+  <si>
+    <t>Refers to the id of the injury code</t>
+  </si>
+  <si>
+    <t>Refers to the id of the report</t>
+  </si>
+  <si>
+    <t>Links the code/s and the report</t>
+  </si>
+  <si>
+    <t>Injury Code</t>
+  </si>
+  <si>
+    <t>A code unique to each type of injury</t>
+  </si>
+  <si>
+    <t>INT/Varchar</t>
   </si>
 </sst>
 </file>
@@ -748,7 +982,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -796,13 +1030,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +1050,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +1087,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -867,10 +1101,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -878,10 +1112,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +1129,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -935,7 +1169,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -944,59 +1178,59 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +1243,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1280,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1057,32 +1291,32 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1095,7 +1329,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1143,56 +1377,56 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1439,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1476,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>162</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1253,35 +1487,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1294,13 +1528,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -1331,7 +1565,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1342,20 +1576,29 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>106</v>
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>107</v>
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1367,14 +1610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D492AB84-46C9-431D-9F54-93710E6866E0}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -1405,7 +1648,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1416,20 +1659,272 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>110</v>
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADFEF55-954C-4D94-9D40-52D04DAD3037}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58480D4B-811D-4010-AEA4-FF0969E380BB}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D950E372-C8A2-4A25-A9A8-4C290B89F6EE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1443,7 +1938,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,7 +1975,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1494,10 +1989,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1511,16 +2006,762 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C3506-B0C9-4983-BDB6-BF2163739F8C}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2A96B2-6EF2-459E-91ED-50BE450E5A4F}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC5D68B-F4FB-41BE-AF0D-F008077028D0}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24472861-FBD5-4E99-910B-33BFEB1F294F}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2708B453-4276-4B0B-9358-A2FC484EA473}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19F32F5-D7DE-48FD-80DC-B47656AB291E}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78166D8D-5512-405D-8AE5-BD7EA6D558B2}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC2BD79-D4BD-42A6-86BA-A85425F80A9C}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61C712F-90AA-4040-87A9-7674EC6199BF}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +2812,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1582,90 +2823,90 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1679,7 +2920,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,7 +2949,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1728,42 +2969,42 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1817,7 +3058,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1828,24 +3069,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +3100,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1896,7 +3137,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1907,24 +3148,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1937,13 +3178,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -1974,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1985,24 +3226,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2016,7 +3257,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2053,7 +3294,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -2064,24 +3305,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2092,15 +3333,15 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D373D72A-ADE9-4F1E-BE71-D18BF2E63DA0}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="45.109375" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
@@ -2132,7 +3373,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -2143,46 +3384,68 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data dictionary acc table
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haysa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CDF6AC-8727-4808-B867-27A671DBFF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB921DE-4301-435F-A132-9DD222A4BB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="20" activeTab="27" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="19" activeTab="27" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
   </bookViews>
   <sheets>
     <sheet name="Role" sheetId="3" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="190">
   <si>
     <t>Key</t>
   </si>
@@ -619,6 +619,18 @@
   </si>
   <si>
     <t>INT/Varchar</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Refers to the injury codes</t>
+  </si>
+  <si>
+    <t>The offices phone number</t>
+  </si>
+  <si>
+    <t>The offices address</t>
   </si>
 </sst>
 </file>
@@ -2710,7 +2722,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,11 +2769,42 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>